<commit_message>
adding role and modify query data by departement
</commit_message>
<xml_diff>
--- a/public/data-attendance/data.xlsx
+++ b/public/data-attendance/data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0475464-1EC7-40AF-A857-CBA7AFDF2471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D027E3-B83D-43A5-91B8-286433801404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{C2091E63-716D-4806-A5B2-25296039E645}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{C2091E63-716D-4806-A5B2-25296039E645}"/>
   </bookViews>
   <sheets>
     <sheet name="M2" sheetId="2" r:id="rId1"/>
     <sheet name="TM" sheetId="3" r:id="rId2"/>
     <sheet name="SM" sheetId="4" r:id="rId3"/>
+    <sheet name="QA" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="342">
   <si>
     <t>1</t>
   </si>
@@ -858,6 +859,201 @@
   </si>
   <si>
     <t xml:space="preserve"> GITA RISKA BR S</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>020513</t>
+  </si>
+  <si>
+    <t>346</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MURHANA</t>
+  </si>
+  <si>
+    <t>200102</t>
+  </si>
+  <si>
+    <t>1598</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DIAN NOVIANTI</t>
+  </si>
+  <si>
+    <t>200121</t>
+  </si>
+  <si>
+    <t>1617</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SITI ZAINAB</t>
+  </si>
+  <si>
+    <t>200204</t>
+  </si>
+  <si>
+    <t>1625</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DEWI RARA N</t>
+  </si>
+  <si>
+    <t>200804</t>
+  </si>
+  <si>
+    <t>1713</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PENI ANGGRAINI</t>
+  </si>
+  <si>
+    <t>201103</t>
+  </si>
+  <si>
+    <t>1724</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MELLYANI</t>
+  </si>
+  <si>
+    <t>201108</t>
+  </si>
+  <si>
+    <t>1729</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MANNA MALAU</t>
+  </si>
+  <si>
+    <t>210502</t>
+  </si>
+  <si>
+    <t>1835</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HAMDANI IKHSAN</t>
+  </si>
+  <si>
+    <t>210707</t>
+  </si>
+  <si>
+    <t>1907</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DEVITA AGNESTI </t>
+  </si>
+  <si>
+    <t>221001</t>
+  </si>
+  <si>
+    <t>2076</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> INDRA MEDA H</t>
+  </si>
+  <si>
+    <t>221006</t>
+  </si>
+  <si>
+    <t>2081</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FEBRYANI SALSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AL</t>
+  </si>
+  <si>
+    <t>221204</t>
+  </si>
+  <si>
+    <t>2088</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MEILIANA DWI P</t>
+  </si>
+  <si>
+    <t>230201</t>
+  </si>
+  <si>
+    <t>2096</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FAJAR ANDIKA B</t>
+  </si>
+  <si>
+    <t>230401</t>
+  </si>
+  <si>
+    <t>2105</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ENDRA DELIMA</t>
+  </si>
+  <si>
+    <t>231001</t>
+  </si>
+  <si>
+    <t>2116</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ENDIKA VIORENT</t>
+  </si>
+  <si>
+    <t>231002</t>
+  </si>
+  <si>
+    <t>2117</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IDA RIANI B R</t>
+  </si>
+  <si>
+    <t>240101</t>
+  </si>
+  <si>
+    <t>2144</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> META DWI K</t>
+  </si>
+  <si>
+    <t>240302</t>
+  </si>
+  <si>
+    <t>2146</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YULIA RAHMAWATI</t>
+  </si>
+  <si>
+    <t>202402</t>
+  </si>
+  <si>
+    <t>2166</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AFLIKAH NURAINI</t>
+  </si>
+  <si>
+    <t>202409</t>
+  </si>
+  <si>
+    <t>2173</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CHIKAL CAROLINE</t>
+  </si>
+  <si>
+    <t>241005</t>
+  </si>
+  <si>
+    <t>2211</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YOLA ARIYANTI</t>
   </si>
 </sst>
 </file>
@@ -1015,18 +1211,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1037,6 +1221,18 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1353,7 +1549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB656625-88DE-46DA-ADC8-1B7B2DEC1FAC}">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
@@ -1368,25 +1564,25 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -1394,14 +1590,14 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -1417,14 +1613,14 @@
       <c r="Q5" s="3"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="32"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1440,54 +1636,54 @@
       <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26" t="s">
+      <c r="H7" s="31"/>
+      <c r="I7" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26" t="s">
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="27" t="s">
+      <c r="P7" s="32"/>
+      <c r="Q7" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="R7" s="27" t="s">
+      <c r="R7" s="23" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
       <c r="G8" s="4" t="s">
         <v>72</v>
       </c>
@@ -1518,8 +1714,8 @@
       <c r="P8" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -3454,14 +3650,14 @@
       <c r="R62" s="9"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A63" s="23" t="s">
+      <c r="A63" s="30" t="s">
         <v>239</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23"/>
-      <c r="F63" s="23"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
       <c r="G63" s="10"/>
       <c r="H63" s="10"/>
       <c r="I63" s="10"/>
@@ -3609,6 +3805,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="O7:P7"/>
     <mergeCell ref="Q7:Q8"/>
     <mergeCell ref="R7:R8"/>
     <mergeCell ref="A2:Q2"/>
@@ -3621,11 +3822,6 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="O7:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3635,7 +3831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B237DAD-584F-41B8-AFE0-311046A29578}">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
@@ -3647,25 +3843,25 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -3673,14 +3869,14 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -3696,14 +3892,14 @@
       <c r="Q5" s="3"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="27" t="s">
         <v>245</v>
       </c>
-      <c r="D6" s="32"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -3719,54 +3915,54 @@
       <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26" t="s">
+      <c r="H7" s="31"/>
+      <c r="I7" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26" t="s">
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="27" t="s">
+      <c r="P7" s="32"/>
+      <c r="Q7" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="R7" s="27" t="s">
+      <c r="R7" s="23" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
       <c r="G8" s="4" t="s">
         <v>72</v>
       </c>
@@ -3797,8 +3993,8 @@
       <c r="P8" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -3909,14 +4105,14 @@
       <c r="R11" s="9"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="30" t="s">
         <v>239</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -4064,6 +4260,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="O7:P7"/>
     <mergeCell ref="Q7:Q8"/>
     <mergeCell ref="R7:R8"/>
     <mergeCell ref="A2:Q2"/>
@@ -4076,11 +4277,6 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="O7:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4090,7 +4286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DE540F-4223-42FF-B935-2A356CDDDFF8}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
@@ -4102,25 +4298,25 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -4128,14 +4324,14 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -4151,14 +4347,14 @@
       <c r="Q5" s="3"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="27" t="s">
         <v>255</v>
       </c>
-      <c r="D6" s="32"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -4174,54 +4370,54 @@
       <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26" t="s">
+      <c r="H7" s="31"/>
+      <c r="I7" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26" t="s">
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="27" t="s">
+      <c r="P7" s="32"/>
+      <c r="Q7" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="R7" s="27" t="s">
+      <c r="R7" s="23" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
       <c r="G8" s="4" t="s">
         <v>72</v>
       </c>
@@ -4252,8 +4448,8 @@
       <c r="P8" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -4504,14 +4700,14 @@
       <c r="R15" s="9"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="30" t="s">
         <v>239</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -4640,7 +4836,1077 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="R7:R8"/>
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="A16:F16"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="O7:P7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84717A58-7BDE-4781-BF82-0DE4AFA8EA24}">
+  <dimension ref="A1:R36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="R1" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="26"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="31"/>
+      <c r="I7" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="R7" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5">
+        <v>2</v>
+      </c>
+      <c r="K8" s="5">
+        <v>3</v>
+      </c>
+      <c r="L8" s="5">
+        <v>4</v>
+      </c>
+      <c r="M8" s="5">
+        <v>5</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D9" s="7">
+        <v>37396</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="9"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D10" s="7">
+        <v>43851</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="8">
+        <v>7</v>
+      </c>
+      <c r="H10" s="8">
+        <v>43</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="9"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D11" s="7">
+        <v>43851</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="8">
+        <v>7</v>
+      </c>
+      <c r="H11" s="8">
+        <v>51</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="9"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D12" s="7">
+        <v>43882</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="8">
+        <v>7</v>
+      </c>
+      <c r="H12" s="8">
+        <v>16</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="9"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D13" s="7">
+        <v>44067</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="9"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D14" s="7">
+        <v>44158</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="8">
+        <v>7</v>
+      </c>
+      <c r="H14" s="8">
+        <v>59</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="9"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D15" s="7">
+        <v>44165</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="8">
+        <v>7</v>
+      </c>
+      <c r="H15" s="8">
+        <v>53</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="9"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D16" s="7">
+        <v>44337</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="8">
+        <v>7</v>
+      </c>
+      <c r="H16" s="8">
+        <v>46</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="9"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D17" s="7">
+        <v>44403</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="8">
+        <v>7</v>
+      </c>
+      <c r="H17" s="8">
+        <v>57</v>
+      </c>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="9"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D18" s="7">
+        <v>44844</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="8">
+        <v>7</v>
+      </c>
+      <c r="H18" s="8">
+        <v>49</v>
+      </c>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="9"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D19" s="7">
+        <v>44855</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="R19" s="9"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D20" s="7">
+        <v>44907</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="8">
+        <v>7</v>
+      </c>
+      <c r="H20" s="8">
+        <v>40</v>
+      </c>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="9"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D21" s="7">
+        <v>44966</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="8">
+        <v>7</v>
+      </c>
+      <c r="H21" s="8">
+        <v>31</v>
+      </c>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="9"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D22" s="7">
+        <v>45020</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="8">
+        <v>7</v>
+      </c>
+      <c r="H22" s="8">
+        <v>49</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="9"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D23" s="7">
+        <v>45202</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="8">
+        <v>7</v>
+      </c>
+      <c r="H23" s="8">
+        <v>20</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="9"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D24" s="7">
+        <v>45212</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="8">
+        <v>7</v>
+      </c>
+      <c r="H24" s="8">
+        <v>54</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="9"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D25" s="7">
+        <v>45306</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="8">
+        <v>7</v>
+      </c>
+      <c r="H25" s="8">
+        <v>53</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="9"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D26" s="7">
+        <v>45372</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="8">
+        <v>7</v>
+      </c>
+      <c r="H26" s="8">
+        <v>56</v>
+      </c>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="9"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D27" s="7">
+        <v>45483</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="8">
+        <v>7</v>
+      </c>
+      <c r="H27" s="8">
+        <v>25</v>
+      </c>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="9"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D28" s="7">
+        <v>45483</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="9"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D29" s="7">
+        <v>45586</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="8">
+        <v>7</v>
+      </c>
+      <c r="H29" s="8">
+        <v>51</v>
+      </c>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="9"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A30" s="30" t="s">
+        <v>239</v>
+      </c>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="9"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="16"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A32" s="16"/>
+      <c r="B32" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E32" s="16"/>
+      <c r="F32" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="16"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="16"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="16"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A35" s="16"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="16"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A36" s="16"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="I36" s="15"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="15"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="A30:F30"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:N7"/>

</xml_diff>